<commit_message>
Resequenced columns on prop bets for better output
File looks better.  Still need to clean up the power-up usage.
</commit_message>
<xml_diff>
--- a/prop_bets.xlsx
+++ b/prop_bets.xlsx
@@ -14,32 +14,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <si>
+    <t>mp</t>
+  </si>
+  <si>
+    <t>foulvictory</t>
+  </si>
   <si>
     <t>autorun</t>
   </si>
   <si>
+    <t>quests</t>
+  </si>
+  <si>
+    <t>climbs</t>
+  </si>
+  <si>
     <t>boss</t>
   </si>
   <si>
-    <t>climbs</t>
-  </si>
-  <si>
-    <t>foulvictory</t>
-  </si>
-  <si>
-    <t>mp</t>
+    <t>puavg</t>
   </si>
   <si>
     <t>powerUp</t>
   </si>
   <si>
-    <t>puavg</t>
-  </si>
-  <si>
-    <t>quests</t>
-  </si>
-  <si>
     <t>gagai</t>
   </si>
   <si>
@@ -106,28 +106,43 @@
     <t>wamou</t>
   </si>
   <si>
-    <t>{'Boost': [47, 12, 13, 22], 'Levitate': 72, 'Force': [25, 11, 9, 5]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [42, 30, 7, 5], 'Levitate': 20, 'Force': [22, 6, 11, 5]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [55, 25, 14, 16], 'Levitate': 70, 'Force': [38, 15, 13, 10]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [66, 19, 29, 18], 'Levitate': 93, 'Force': [44, 13, 22, 9]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [20, 12, 3, 5], 'Levitate': 24, 'Force': [5, 2, 2, 1]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [52, 23, 10, 19], 'Levitate': 76, 'Force': [30, 11, 12, 7]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [49, 23, 13, 13], 'Levitate': 62, 'Force': [22, 9, 6, 7]}</t>
-  </si>
-  <si>
-    <t>{'Boost': [47, 28, 5, 14], 'Levitate': 61, 'Force': [36, 9, 16, 11]}</t>
+    <t>{'Levitate': 102, 'Force': [50, 18, 20, 12], 'Boost': [69, 31, 18, 20]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 105, 'Force': [38, 14, 15, 9], 'Boost': [80, 23, 19, 38]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 20, 'Force': [22, 6, 11, 5], 'Boost': [42, 30, 7, 5]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 119, 'Force': [63, 24, 20, 19], 'Boost': [93, 40, 22, 31]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 121, 'Force': [60, 17, 19, 24], 'Boost': [65, 16, 17, 32]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 138, 'Force': [64, 20, 30, 14], 'Boost': [101, 33, 38, 30]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 84, 'Force': [43, 14, 21, 8], 'Boost': [62, 22, 17, 23]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 84, 'Force': [26, 10, 10, 6], 'Boost': [64, 30, 10, 24]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 117, 'Force': [46, 15, 22, 9], 'Boost': [78, 33, 10, 35]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 62, 'Force': [22, 9, 6, 7], 'Boost': [49, 23, 13, 13]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 99, 'Force': [59, 14, 26, 19], 'Boost': [80, 46, 9, 25]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 24, 'Force': [9, 4, 4, 1], 'Boost': [17, 6, 7, 4]}</t>
+  </si>
+  <si>
+    <t>{'Levitate': 97, 'Force': [38, 10, 17, 11], 'Boost': [73, 35, 17, 21]}</t>
   </si>
 </sst>
 </file>
@@ -521,6 +536,30 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+      <c r="D2">
+        <v>4.25</v>
+      </c>
+      <c r="E2">
+        <v>0.35</v>
+      </c>
+      <c r="F2">
+        <v>0.3875</v>
+      </c>
+      <c r="G2">
+        <v>0.0125</v>
+      </c>
+      <c r="H2">
+        <v>2.7625</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
@@ -552,28 +591,28 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>4.47272727272727</v>
+        <v>80</v>
       </c>
       <c r="C8">
-        <v>0.0545454545454545</v>
+        <v>0.0375</v>
       </c>
       <c r="D8">
-        <v>0.854545454545454</v>
+        <v>4.625</v>
       </c>
       <c r="E8">
-        <v>0.0181818181818182</v>
+        <v>0.425</v>
       </c>
       <c r="F8">
-        <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
+        <v>0.8</v>
+      </c>
+      <c r="G8">
+        <v>0.0375</v>
       </c>
       <c r="H8">
-        <v>2.61818181818182</v>
-      </c>
-      <c r="I8">
-        <v>0.345454545454545</v>
+        <v>2.7875</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -581,28 +620,28 @@
         <v>15</v>
       </c>
       <c r="B9">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>0.0571428571428571</v>
+      </c>
+      <c r="D9">
         <v>3.25714285714286</v>
       </c>
-      <c r="C9">
+      <c r="E9">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="F9">
+        <v>0.257142857142857</v>
+      </c>
+      <c r="G9">
         <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0.257142857142857</v>
-      </c>
-      <c r="E9">
-        <v>0.0571428571428571</v>
-      </c>
-      <c r="F9">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
       </c>
       <c r="H9">
         <v>2.4</v>
       </c>
-      <c r="I9">
-        <v>0.114285714285714</v>
+      <c r="I9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -610,28 +649,28 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>4.88461538461539</v>
+        <v>87</v>
       </c>
       <c r="C10">
-        <v>0.230769230769231</v>
+        <v>0.0689655172413793</v>
       </c>
       <c r="D10">
-        <v>1.30769230769231</v>
+        <v>5.06896551724138</v>
       </c>
       <c r="E10">
-        <v>0.0769230769230769</v>
+        <v>0.850574712643678</v>
       </c>
       <c r="F10">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
+        <v>1.27586206896552</v>
+      </c>
+      <c r="G10">
+        <v>0.218390804597701</v>
       </c>
       <c r="H10">
-        <v>3.13461538461538</v>
-      </c>
-      <c r="I10">
-        <v>0.788461538461538</v>
+        <v>3.16091954022989</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -643,40 +682,88 @@
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>0.0428571428571429</v>
+      </c>
+      <c r="D12">
+        <v>5.44285714285714</v>
+      </c>
+      <c r="E12">
+        <v>1.2</v>
+      </c>
+      <c r="F12">
+        <v>1.35714285714286</v>
+      </c>
+      <c r="G12">
+        <v>0.0857142857142857</v>
+      </c>
+      <c r="H12">
+        <v>3.51428571428571</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13">
-        <v>5.18461538461538</v>
+        <v>92</v>
       </c>
       <c r="C13">
-        <v>0.0769230769230769</v>
+        <v>0.0434782608695652</v>
       </c>
       <c r="D13">
-        <v>1.24615384615385</v>
+        <v>5.35869565217391</v>
       </c>
       <c r="E13">
-        <v>0.0461538461538462</v>
+        <v>0.967391304347826</v>
       </c>
       <c r="F13">
-        <v>65</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
+        <v>1.30434782608696</v>
+      </c>
+      <c r="G13">
+        <v>0.0978260869565217</v>
       </c>
       <c r="H13">
-        <v>3.12307692307692</v>
-      </c>
-      <c r="I13">
-        <v>0.830769230769231</v>
+        <v>3.29347826086957</v>
+      </c>
+      <c r="I13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B14">
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>4.98214285714286</v>
+      </c>
+      <c r="E14">
+        <v>0.589285714285714</v>
+      </c>
+      <c r="F14">
+        <v>0.928571428571429</v>
+      </c>
+      <c r="G14">
+        <v>0.0892857142857143</v>
+      </c>
+      <c r="H14">
+        <v>3.375</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
@@ -688,28 +775,28 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>3.77272727272727</v>
+        <v>74</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.0540540540540541</v>
       </c>
       <c r="D16">
-        <v>0.454545454545455</v>
+        <v>4.58108108108108</v>
       </c>
       <c r="E16">
-        <v>0.0909090909090909</v>
+        <v>0.689189189189189</v>
       </c>
       <c r="F16">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
+        <v>0.689189189189189</v>
+      </c>
+      <c r="G16">
+        <v>0.0405405405405405</v>
       </c>
       <c r="H16">
-        <v>2.22727272727273</v>
-      </c>
-      <c r="I16">
-        <v>0.363636363636364</v>
+        <v>2.35135135135135</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -722,28 +809,28 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>4.52542372881356</v>
+        <v>83</v>
       </c>
       <c r="C18">
-        <v>0.0847457627118644</v>
+        <v>0.0843373493975904</v>
       </c>
       <c r="D18">
-        <v>1.10169491525424</v>
+        <v>4.79518072289157</v>
       </c>
       <c r="E18">
-        <v>0.101694915254237</v>
+        <v>0.578313253012048</v>
       </c>
       <c r="F18">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>35</v>
+        <v>1.32530120481928</v>
+      </c>
+      <c r="G18">
+        <v>0.156626506024096</v>
       </c>
       <c r="H18">
-        <v>2.67796610169492</v>
-      </c>
-      <c r="I18">
-        <v>0.457627118644068</v>
+        <v>2.90361445783133</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -751,28 +838,28 @@
         <v>25</v>
       </c>
       <c r="B19">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>0.0163934426229508</v>
+      </c>
+      <c r="D19">
         <v>4.72131147540984</v>
       </c>
-      <c r="C19">
+      <c r="E19">
+        <v>0.524590163934426</v>
+      </c>
+      <c r="F19">
+        <v>0.934426229508197</v>
+      </c>
+      <c r="G19">
         <v>0.0491803278688525</v>
-      </c>
-      <c r="D19">
-        <v>0.934426229508197</v>
-      </c>
-      <c r="E19">
-        <v>0.0163934426229508</v>
-      </c>
-      <c r="F19">
-        <v>61</v>
-      </c>
-      <c r="G19" t="s">
-        <v>36</v>
       </c>
       <c r="H19">
         <v>2.18032786885246</v>
       </c>
-      <c r="I19">
-        <v>0.524590163934426</v>
+      <c r="I19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -785,38 +872,86 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>4.98076923076923</v>
+        <v>78</v>
       </c>
       <c r="C21">
-        <v>0.115384615384615</v>
+        <v>0.0256410256410256</v>
       </c>
       <c r="D21">
-        <v>0.865384615384615</v>
+        <v>5.12820512820513</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="F21">
-        <v>52</v>
-      </c>
-      <c r="G21" t="s">
-        <v>37</v>
+        <v>0.884615384615385</v>
+      </c>
+      <c r="G21">
+        <v>0.102564102564103</v>
       </c>
       <c r="H21">
-        <v>2.76923076923077</v>
-      </c>
-      <c r="I21">
-        <v>0.461538461538462</v>
+        <v>3.05128205128205</v>
+      </c>
+      <c r="I21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>0.0476190476190476</v>
+      </c>
+      <c r="D22">
+        <v>3.47619047619048</v>
+      </c>
+      <c r="E22">
+        <v>0.380952380952381</v>
+      </c>
+      <c r="F22">
+        <v>0.428571428571429</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2.38095238095238</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B23">
+        <v>78</v>
+      </c>
+      <c r="C23">
+        <v>0.0128205128205128</v>
+      </c>
+      <c r="D23">
+        <v>5.01282051282051</v>
+      </c>
+      <c r="E23">
+        <v>0.807692307692308</v>
+      </c>
+      <c r="F23">
+        <v>0.769230769230769</v>
+      </c>
+      <c r="G23">
+        <v>0.0641025641025641</v>
+      </c>
+      <c r="H23">
+        <v>2.66666666666667</v>
+      </c>
+      <c r="I23" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>